<commit_message>
Modified the git functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/AutomationCreation.xlsx
+++ b/src/test/resources/excel/AutomationCreation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="14484" windowHeight="3864" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="14484" windowHeight="3864"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>vaibhav.nathe@rediffmail.com</t>
+  </si>
+  <si>
+    <t>StartDaystoAdd</t>
+  </si>
+  <si>
+    <t>EnddaystoAdd</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -105,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -116,6 +131,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,8 +455,14 @@
       <c r="D1" t="s">
         <v>10</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -453,8 +475,14 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -466,10 +494,17 @@
       </c>
       <c r="D3" t="s">
         <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -477,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>